<commit_message>
working home for evmc
</commit_message>
<xml_diff>
--- a/data/raw-data/raw-ticks/collect/20250505_collect_tick.xlsx
+++ b/data/raw-data/raw-ticks/collect/20250505_collect_tick.xlsx
@@ -11,7 +11,7 @@
     <sheet name="verif juin" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="163">
   <si>
     <t>date</t>
   </si>
@@ -526,6 +526,21 @@
   </si>
   <si>
     <t>1 tique</t>
+  </si>
+  <si>
+    <t>month_year</t>
+  </si>
+  <si>
+    <t>Juin_2023</t>
+  </si>
+  <si>
+    <t>Juin_2024</t>
+  </si>
+  <si>
+    <t>Octobre_2023</t>
+  </si>
+  <si>
+    <t>Septembre_2024</t>
   </si>
 </sst>
 </file>
@@ -857,2945 +872,3448 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F184"/>
+  <dimension ref="A1:G184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="J122" sqref="J122"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="1" max="2" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>100</v>
       </c>
       <c r="B1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>45078</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>45078</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>45085</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>45085</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>45085</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>45085</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>45085</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>45085</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>45085</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>45078</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>45085</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>45078</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>24</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>45085</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>45085</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>45085</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>45085</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>45085</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>45085</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
       <c r="B20" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>45085</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
       <c r="B21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>45085</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>9</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
       <c r="B22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C22" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>45085</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <v>45085</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
       <c r="B24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>45078</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>12</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>45085</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>159</v>
+      </c>
+      <c r="C26" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <v>45085</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>6</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
       <c r="B27" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>45085</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
       <c r="B28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>45081</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>6</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
       <c r="B29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>45081</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
       <c r="B30" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>45081</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
       <c r="B31" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>45078</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
       <c r="B32" t="s">
+        <v>159</v>
+      </c>
+      <c r="C32" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>45078</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>8</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>45078</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>2</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>
       <c r="B34" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D34" s="1">
         <v>45078</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>21</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2</v>
       </c>
       <c r="B35" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <v>45078</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
       <c r="B36" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D36" s="1">
         <v>45078</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>19</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
       <c r="B37" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="1">
+      <c r="D37" s="1">
         <v>45455</v>
       </c>
-      <c r="D37">
-        <v>4</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="G37" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
       <c r="B38" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="1">
+      <c r="D38" s="1">
         <v>45458</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>4</v>
       </c>
       <c r="B39" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D39" s="1">
         <v>45458</v>
       </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
       <c r="B40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="1">
+      <c r="D40" s="1">
         <v>45458</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
       <c r="B41" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="1">
+      <c r="D41" s="1">
         <v>45458</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>4</v>
       </c>
       <c r="B42" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="1">
+      <c r="D42" s="1">
         <v>45459</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>2</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>4</v>
       </c>
       <c r="B43" t="s">
+        <v>160</v>
+      </c>
+      <c r="C43" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="1">
+      <c r="D43" s="1">
         <v>45458</v>
       </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4</v>
       </c>
       <c r="B44" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="1">
+      <c r="D44" s="1">
         <v>45458</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4</v>
       </c>
       <c r="B45" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="1">
+      <c r="D45" s="1">
         <v>45464</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
       <c r="B46" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="1">
+      <c r="D46" s="1">
         <v>45464</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>4</v>
       </c>
       <c r="B47" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="1">
+      <c r="D47" s="1">
         <v>45455</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>3</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4</v>
       </c>
       <c r="B48" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="1">
+      <c r="D48" s="1">
         <v>45464</v>
       </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
       <c r="B49" t="s">
+        <v>160</v>
+      </c>
+      <c r="C49" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="1">
+      <c r="D49" s="1">
         <v>45464</v>
       </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
       <c r="B50" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="1">
+      <c r="D50" s="1">
         <v>45464</v>
       </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="G50" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
       <c r="B51" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="1">
+      <c r="D51" s="1">
         <v>45464</v>
       </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
       <c r="B52" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="1">
+      <c r="D52" s="1">
         <v>45464</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>4</v>
       </c>
       <c r="B53" t="s">
+        <v>160</v>
+      </c>
+      <c r="C53" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="1">
+      <c r="D53" s="1">
         <v>45461</v>
       </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="G53" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>4</v>
       </c>
       <c r="B54" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="1">
+      <c r="D54" s="1">
         <v>45461</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>3</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>4</v>
       </c>
       <c r="B55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="1">
+      <c r="D55" s="1">
         <v>45461</v>
       </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="G55" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>4</v>
       </c>
       <c r="B56" t="s">
+        <v>160</v>
+      </c>
+      <c r="C56" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="1">
+      <c r="D56" s="1">
         <v>45461</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>5</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>4</v>
       </c>
       <c r="B57" t="s">
+        <v>160</v>
+      </c>
+      <c r="C57" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="1">
+      <c r="D57" s="1">
         <v>45455</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>5</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>4</v>
       </c>
       <c r="B58" t="s">
+        <v>160</v>
+      </c>
+      <c r="C58" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="1">
+      <c r="D58" s="1">
         <v>45461</v>
       </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="G58" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>4</v>
       </c>
       <c r="B59" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" t="s">
         <v>41</v>
       </c>
-      <c r="C59" s="1">
+      <c r="D59" s="1">
         <v>45460</v>
       </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="G59" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>4</v>
       </c>
       <c r="B60" t="s">
+        <v>160</v>
+      </c>
+      <c r="C60" t="s">
         <v>38</v>
       </c>
-      <c r="C60" s="1">
+      <c r="D60" s="1">
         <v>45461</v>
       </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="G60" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>4</v>
       </c>
       <c r="B61" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" t="s">
         <v>39</v>
       </c>
-      <c r="C61" s="1">
+      <c r="D61" s="1">
         <v>45461</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>2</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>4</v>
       </c>
       <c r="B62" t="s">
+        <v>160</v>
+      </c>
+      <c r="C62" t="s">
         <v>40</v>
       </c>
-      <c r="C62" s="1">
+      <c r="D62" s="1">
         <v>45461</v>
       </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="G62" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>4</v>
       </c>
       <c r="B63" t="s">
+        <v>160</v>
+      </c>
+      <c r="C63" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="1">
+      <c r="D63" s="1">
         <v>45458</v>
       </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>4</v>
       </c>
       <c r="B64" t="s">
+        <v>160</v>
+      </c>
+      <c r="C64" t="s">
         <v>57</v>
       </c>
-      <c r="C64" s="1">
+      <c r="D64" s="1">
         <v>45458</v>
       </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="G64" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>4</v>
       </c>
       <c r="B65" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" t="s">
         <v>66</v>
       </c>
-      <c r="C65" s="1">
+      <c r="D65" s="1">
         <v>45455</v>
       </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="G65" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>4</v>
       </c>
       <c r="B66" t="s">
+        <v>160</v>
+      </c>
+      <c r="C66" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="1">
+      <c r="D66" s="1">
         <v>45458</v>
       </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="G66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>4</v>
       </c>
       <c r="B67" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" t="s">
         <v>44</v>
       </c>
-      <c r="C67" s="1">
+      <c r="D67" s="1">
         <v>45460</v>
       </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="G67" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>4</v>
       </c>
       <c r="B68" t="s">
+        <v>160</v>
+      </c>
+      <c r="C68" t="s">
         <v>46</v>
       </c>
-      <c r="C68" s="1">
+      <c r="D68" s="1">
         <v>45460</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>2</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>4</v>
       </c>
       <c r="B69" t="s">
+        <v>160</v>
+      </c>
+      <c r="C69" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="1">
+      <c r="D69" s="1">
         <v>45463</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>3</v>
       </c>
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>4</v>
       </c>
       <c r="B70" t="s">
+        <v>160</v>
+      </c>
+      <c r="C70" t="s">
         <v>19</v>
       </c>
-      <c r="C70" s="1">
+      <c r="D70" s="1">
         <v>45463</v>
       </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="G70" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>4</v>
       </c>
       <c r="B71" t="s">
+        <v>160</v>
+      </c>
+      <c r="C71" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="1">
+      <c r="D71" s="1">
         <v>45463</v>
       </c>
-      <c r="D71">
+      <c r="E71">
         <v>12</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>4</v>
       </c>
       <c r="B72" t="s">
+        <v>160</v>
+      </c>
+      <c r="C72" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="1">
+      <c r="D72" s="1">
         <v>45455</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <v>3</v>
       </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>4</v>
       </c>
       <c r="B73" t="s">
+        <v>160</v>
+      </c>
+      <c r="C73" t="s">
         <v>23</v>
       </c>
-      <c r="C73" s="1">
+      <c r="D73" s="1">
         <v>45463</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <v>12</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>4</v>
       </c>
       <c r="B74" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" t="s">
         <v>24</v>
       </c>
-      <c r="C74" s="1">
+      <c r="D74" s="1">
         <v>45463</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <v>3</v>
       </c>
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>4</v>
       </c>
       <c r="B75" t="s">
+        <v>160</v>
+      </c>
+      <c r="C75" t="s">
         <v>26</v>
       </c>
-      <c r="C75" s="1">
+      <c r="D75" s="1">
         <v>45463</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <v>10</v>
       </c>
-      <c r="F75" t="s">
+      <c r="G75" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>4</v>
       </c>
       <c r="B76" t="s">
+        <v>160</v>
+      </c>
+      <c r="C76" t="s">
         <v>28</v>
       </c>
-      <c r="C76" s="1">
+      <c r="D76" s="1">
         <v>45463</v>
       </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="G76" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>4</v>
       </c>
       <c r="B77" t="s">
+        <v>160</v>
+      </c>
+      <c r="C77" t="s">
         <v>60</v>
       </c>
-      <c r="C77" s="1">
+      <c r="D77" s="1">
         <v>45458</v>
       </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-      <c r="F77" t="s">
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="G77" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>4</v>
       </c>
       <c r="B78" t="s">
+        <v>160</v>
+      </c>
+      <c r="C78" t="s">
         <v>68</v>
       </c>
-      <c r="C78" s="1">
+      <c r="D78" s="1">
         <v>45455</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <v>3</v>
       </c>
-      <c r="F78" t="s">
+      <c r="G78" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>4</v>
       </c>
       <c r="B79" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" t="s">
         <v>69</v>
       </c>
-      <c r="C79" s="1">
+      <c r="D79" s="1">
         <v>45455</v>
       </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="F79" t="s">
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="G79" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>4</v>
       </c>
       <c r="B80" t="s">
+        <v>160</v>
+      </c>
+      <c r="C80" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="1">
+      <c r="D80" s="1">
         <v>45455</v>
       </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-      <c r="F80" t="s">
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="G80" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1</v>
       </c>
       <c r="B81" t="s">
+        <v>161</v>
+      </c>
+      <c r="C81" t="s">
         <v>62</v>
       </c>
-      <c r="C81" s="1">
+      <c r="D81" s="1">
         <v>45216</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>2</v>
       </c>
-      <c r="F81" t="s">
+      <c r="G81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1</v>
       </c>
       <c r="B82" t="s">
+        <v>161</v>
+      </c>
+      <c r="C82" t="s">
         <v>48</v>
       </c>
-      <c r="C82" s="1">
+      <c r="D82" s="1">
         <v>45216</v>
       </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="G82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1</v>
       </c>
       <c r="B83" t="s">
+        <v>161</v>
+      </c>
+      <c r="C83" t="s">
         <v>50</v>
       </c>
-      <c r="C83" s="1">
+      <c r="D83" s="1">
         <v>45221</v>
       </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="F83" t="s">
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="G83" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1</v>
       </c>
       <c r="B84" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" t="s">
         <v>51</v>
       </c>
-      <c r="C84" s="1">
+      <c r="D84" s="1">
         <v>45221</v>
       </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="G84" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1</v>
       </c>
       <c r="B85" t="s">
+        <v>161</v>
+      </c>
+      <c r="C85" t="s">
         <v>52</v>
       </c>
-      <c r="C85" s="1">
+      <c r="D85" s="1">
         <v>45221</v>
       </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="G85" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1</v>
       </c>
       <c r="B86" t="s">
+        <v>161</v>
+      </c>
+      <c r="C86" t="s">
         <v>76</v>
       </c>
-      <c r="C86" s="1">
+      <c r="D86" s="1">
         <v>45221</v>
       </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="G86" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1</v>
       </c>
       <c r="B87" t="s">
+        <v>161</v>
+      </c>
+      <c r="C87" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="1">
+      <c r="D87" s="1">
         <v>45221</v>
       </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="G87" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1</v>
       </c>
       <c r="B88" t="s">
+        <v>161</v>
+      </c>
+      <c r="C88" t="s">
         <v>53</v>
       </c>
-      <c r="C88" s="1">
+      <c r="D88" s="1">
         <v>45221</v>
       </c>
-      <c r="D88">
-        <v>0</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="G88" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1</v>
       </c>
       <c r="B89" t="s">
+        <v>161</v>
+      </c>
+      <c r="C89" t="s">
         <v>54</v>
       </c>
-      <c r="C89" s="1">
+      <c r="D89" s="1">
         <v>45221</v>
       </c>
-      <c r="D89">
-        <v>0</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="G89" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1</v>
       </c>
       <c r="B90" t="s">
+        <v>161</v>
+      </c>
+      <c r="C90" t="s">
         <v>7</v>
       </c>
-      <c r="C90" s="1">
+      <c r="D90" s="1">
         <v>45216</v>
       </c>
-      <c r="D90">
-        <v>1</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="G90" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1</v>
       </c>
       <c r="B91" t="s">
+        <v>161</v>
+      </c>
+      <c r="C91" t="s">
         <v>9</v>
       </c>
-      <c r="C91" s="1">
+      <c r="D91" s="1">
         <v>45224</v>
       </c>
-      <c r="D91">
-        <v>0</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="G91" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1</v>
       </c>
       <c r="B92" t="s">
+        <v>161</v>
+      </c>
+      <c r="C92" t="s">
         <v>63</v>
       </c>
-      <c r="C92" s="1">
+      <c r="D92" s="1">
         <v>45216</v>
       </c>
-      <c r="D92">
-        <v>0</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="G92" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1</v>
       </c>
       <c r="B93" t="s">
+        <v>161</v>
+      </c>
+      <c r="C93" t="s">
         <v>11</v>
       </c>
-      <c r="C93" s="1">
+      <c r="D93" s="1">
         <v>45224</v>
       </c>
-      <c r="D93">
-        <v>0</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="G93" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1</v>
       </c>
       <c r="B94" t="s">
+        <v>161</v>
+      </c>
+      <c r="C94" t="s">
         <v>12</v>
       </c>
-      <c r="C94" s="1">
+      <c r="D94" s="1">
         <v>45221</v>
       </c>
-      <c r="D94">
-        <v>0</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="G94" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1</v>
       </c>
       <c r="B95" t="s">
+        <v>161</v>
+      </c>
+      <c r="C95" t="s">
         <v>13</v>
       </c>
-      <c r="C95" s="1">
+      <c r="D95" s="1">
         <v>45221</v>
       </c>
-      <c r="D95">
-        <v>0</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="G95" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1</v>
       </c>
       <c r="B96" t="s">
+        <v>161</v>
+      </c>
+      <c r="C96" t="s">
         <v>14</v>
       </c>
-      <c r="C96" s="1">
+      <c r="D96" s="1">
         <v>45221</v>
       </c>
-      <c r="D96">
-        <v>1</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="G96" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1</v>
       </c>
       <c r="B97" t="s">
+        <v>161</v>
+      </c>
+      <c r="C97" t="s">
         <v>16</v>
       </c>
-      <c r="C97" s="1">
+      <c r="D97" s="1">
         <v>45221</v>
       </c>
-      <c r="D97">
-        <v>0</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="G97" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1</v>
       </c>
       <c r="B98" t="s">
+        <v>161</v>
+      </c>
+      <c r="C98" t="s">
         <v>79</v>
       </c>
-      <c r="C98" s="1">
+      <c r="D98" s="1">
         <v>45221</v>
       </c>
-      <c r="D98">
-        <v>0</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="G98" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1</v>
       </c>
       <c r="B99" t="s">
+        <v>161</v>
+      </c>
+      <c r="C99" t="s">
         <v>30</v>
       </c>
-      <c r="C99" s="1">
+      <c r="D99" s="1">
         <v>45224</v>
       </c>
-      <c r="D99">
-        <v>0</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="G99" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1</v>
       </c>
       <c r="B100" t="s">
+        <v>161</v>
+      </c>
+      <c r="C100" t="s">
         <v>32</v>
       </c>
-      <c r="C100" s="1">
+      <c r="D100" s="1">
         <v>45224</v>
       </c>
-      <c r="D100">
-        <v>0</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="G100" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>1</v>
       </c>
       <c r="B101" t="s">
+        <v>161</v>
+      </c>
+      <c r="C101" t="s">
         <v>34</v>
       </c>
-      <c r="C101" s="1">
+      <c r="D101" s="1">
         <v>45224</v>
       </c>
-      <c r="D101">
-        <v>0</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="G101" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>1</v>
       </c>
       <c r="B102" t="s">
+        <v>161</v>
+      </c>
+      <c r="C102" t="s">
         <v>35</v>
       </c>
-      <c r="C102" s="1">
+      <c r="D102" s="1">
         <v>45224</v>
       </c>
-      <c r="D102">
-        <v>0</v>
-      </c>
-      <c r="F102" t="s">
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="G102" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>1</v>
       </c>
       <c r="B103" t="s">
+        <v>161</v>
+      </c>
+      <c r="C103" t="s">
         <v>65</v>
       </c>
-      <c r="C103" s="1">
+      <c r="D103" s="1">
         <v>45216</v>
       </c>
-      <c r="D103">
-        <v>0</v>
-      </c>
-      <c r="F103" t="s">
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="G103" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1</v>
       </c>
       <c r="B104" t="s">
+        <v>161</v>
+      </c>
+      <c r="C104" t="s">
         <v>37</v>
       </c>
-      <c r="C104" s="1">
+      <c r="D104" s="1">
         <v>45223</v>
       </c>
-      <c r="D104">
-        <v>0</v>
-      </c>
-      <c r="F104" t="s">
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="G104" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1</v>
       </c>
       <c r="B105" t="s">
+        <v>161</v>
+      </c>
+      <c r="C105" t="s">
         <v>41</v>
       </c>
-      <c r="C105" s="1">
+      <c r="D105" s="1">
         <v>45223</v>
       </c>
-      <c r="D105">
-        <v>0</v>
-      </c>
-      <c r="F105" t="s">
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="G105" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1</v>
       </c>
       <c r="B106" t="s">
+        <v>161</v>
+      </c>
+      <c r="C106" t="s">
         <v>38</v>
       </c>
-      <c r="C106" s="1">
+      <c r="D106" s="1">
         <v>45223</v>
       </c>
-      <c r="D106">
-        <v>0</v>
-      </c>
-      <c r="F106" t="s">
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="G106" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1</v>
       </c>
       <c r="B107" t="s">
+        <v>161</v>
+      </c>
+      <c r="C107" t="s">
         <v>39</v>
       </c>
-      <c r="C107" s="1">
+      <c r="D107" s="1">
         <v>45223</v>
       </c>
-      <c r="D107">
-        <v>0</v>
-      </c>
-      <c r="F107" t="s">
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="G107" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1</v>
       </c>
       <c r="B108" t="s">
+        <v>161</v>
+      </c>
+      <c r="C108" t="s">
         <v>40</v>
       </c>
-      <c r="C108" s="1">
+      <c r="D108" s="1">
         <v>45223</v>
       </c>
-      <c r="D108">
-        <v>0</v>
-      </c>
-      <c r="F108" t="s">
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="G108" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1</v>
       </c>
       <c r="B109" t="s">
+        <v>161</v>
+      </c>
+      <c r="C109" t="s">
         <v>74</v>
       </c>
-      <c r="C109" s="1">
+      <c r="D109" s="1">
         <v>45223</v>
       </c>
-      <c r="D109">
-        <v>0</v>
-      </c>
-      <c r="F109" t="s">
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="G109" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1</v>
       </c>
       <c r="B110" t="s">
+        <v>161</v>
+      </c>
+      <c r="C110" t="s">
         <v>55</v>
       </c>
-      <c r="C110" s="1">
+      <c r="D110" s="1">
         <v>45216</v>
       </c>
-      <c r="D110">
-        <v>0</v>
-      </c>
-      <c r="F110" t="s">
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="G110" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1</v>
       </c>
       <c r="B111" t="s">
+        <v>161</v>
+      </c>
+      <c r="C111" t="s">
         <v>66</v>
       </c>
-      <c r="C111" s="1">
+      <c r="D111" s="1">
         <v>45216</v>
       </c>
-      <c r="D111">
-        <v>1</v>
-      </c>
-      <c r="F111" t="s">
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="G111" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1</v>
       </c>
       <c r="B112" t="s">
+        <v>161</v>
+      </c>
+      <c r="C112" t="s">
         <v>67</v>
       </c>
-      <c r="C112" s="1">
+      <c r="D112" s="1">
         <v>45216</v>
       </c>
-      <c r="D112">
-        <v>0</v>
-      </c>
-      <c r="F112" t="s">
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="G112" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>1</v>
       </c>
       <c r="B113" t="s">
+        <v>161</v>
+      </c>
+      <c r="C113" t="s">
         <v>60</v>
       </c>
-      <c r="C113" s="1">
+      <c r="D113" s="1">
         <v>45216</v>
       </c>
-      <c r="D113">
-        <v>0</v>
-      </c>
-      <c r="F113" t="s">
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="G113" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>1</v>
       </c>
       <c r="B114" t="s">
+        <v>161</v>
+      </c>
+      <c r="C114" t="s">
         <v>68</v>
       </c>
-      <c r="C114" s="1">
+      <c r="D114" s="1">
         <v>45216</v>
       </c>
-      <c r="D114">
-        <v>0</v>
-      </c>
-      <c r="F114" t="s">
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="G114" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>1</v>
       </c>
       <c r="B115" t="s">
+        <v>161</v>
+      </c>
+      <c r="C115" t="s">
         <v>69</v>
       </c>
-      <c r="C115" s="1">
+      <c r="D115" s="1">
         <v>45216</v>
       </c>
-      <c r="D115">
-        <v>0</v>
-      </c>
-      <c r="F115" t="s">
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="G115" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>1</v>
       </c>
       <c r="B116" t="s">
+        <v>161</v>
+      </c>
+      <c r="C116" t="s">
         <v>71</v>
       </c>
-      <c r="C116" s="1">
+      <c r="D116" s="1">
         <v>45216</v>
       </c>
-      <c r="D116">
-        <v>0</v>
-      </c>
-      <c r="F116" t="s">
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="G116" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B117" s="4">
+      <c r="B117" t="s">
+        <v>160</v>
+      </c>
+      <c r="C117" s="4">
         <v>14</v>
       </c>
-      <c r="C117" s="5">
+      <c r="D117" s="5">
         <v>45458</v>
       </c>
-      <c r="D117" s="4"/>
       <c r="E117" s="4"/>
-      <c r="F117" s="4" t="e">
+      <c r="F117" s="4"/>
+      <c r="G117" s="4" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B118" s="4">
+      <c r="B118" t="s">
+        <v>160</v>
+      </c>
+      <c r="C118" s="4">
         <v>35</v>
       </c>
-      <c r="C118" s="5">
+      <c r="D118" s="5">
         <v>45491</v>
       </c>
-      <c r="D118" s="4"/>
       <c r="E118" s="4"/>
-      <c r="F118" s="4" t="e">
+      <c r="F118" s="4"/>
+      <c r="G118" s="4" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>103</v>
       </c>
       <c r="B119" t="s">
+        <v>162</v>
+      </c>
+      <c r="C119" t="s">
         <v>62</v>
       </c>
-      <c r="C119" s="1">
+      <c r="D119" s="1">
         <v>45560</v>
       </c>
-      <c r="D119">
-        <v>0</v>
-      </c>
-      <c r="F119" t="s">
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="G119" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>103</v>
       </c>
       <c r="B120" t="s">
+        <v>162</v>
+      </c>
+      <c r="C120" t="s">
         <v>48</v>
       </c>
-      <c r="C120" s="1">
+      <c r="D120" s="1">
         <v>45563</v>
       </c>
-      <c r="D120">
-        <v>0</v>
-      </c>
-      <c r="F120" t="s">
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="G120" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>103</v>
       </c>
       <c r="B121" t="s">
+        <v>162</v>
+      </c>
+      <c r="C121" t="s">
         <v>50</v>
       </c>
-      <c r="C121" s="1">
+      <c r="D121" s="1">
         <v>45563</v>
       </c>
-      <c r="D121">
-        <v>0</v>
-      </c>
-      <c r="F121" t="s">
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="G121" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>103</v>
       </c>
       <c r="B122" t="s">
+        <v>162</v>
+      </c>
+      <c r="C122" t="s">
         <v>51</v>
       </c>
-      <c r="C122" s="1">
+      <c r="D122" s="1">
         <v>45563</v>
       </c>
-      <c r="D122">
-        <v>0</v>
-      </c>
-      <c r="F122" t="s">
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="G122" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>103</v>
       </c>
       <c r="B123" t="s">
+        <v>162</v>
+      </c>
+      <c r="C123" t="s">
         <v>52</v>
       </c>
-      <c r="C123" s="1">
+      <c r="D123" s="1">
         <v>45563</v>
       </c>
-      <c r="D123">
-        <v>0</v>
-      </c>
-      <c r="F123" t="s">
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="G123" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>103</v>
       </c>
       <c r="B124" t="s">
+        <v>162</v>
+      </c>
+      <c r="C124" t="s">
         <v>76</v>
       </c>
-      <c r="C124" s="1">
+      <c r="D124" s="1">
         <v>45569</v>
       </c>
-      <c r="D124">
-        <v>0</v>
-      </c>
-      <c r="F124" t="s">
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="G124" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>103</v>
       </c>
       <c r="B125" t="s">
+        <v>162</v>
+      </c>
+      <c r="C125" t="s">
         <v>5</v>
       </c>
-      <c r="C125" s="1">
+      <c r="D125" s="1">
         <v>45592</v>
       </c>
-      <c r="D125">
-        <v>1</v>
-      </c>
-      <c r="F125" t="s">
+      <c r="E125">
+        <v>1</v>
+      </c>
+      <c r="G125" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>103</v>
       </c>
       <c r="B126" t="s">
+        <v>162</v>
+      </c>
+      <c r="C126" t="s">
         <v>53</v>
       </c>
-      <c r="C126" s="1">
+      <c r="D126" s="1">
         <v>45563</v>
       </c>
-      <c r="D126">
-        <v>0</v>
-      </c>
-      <c r="F126" t="s">
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="G126" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>103</v>
       </c>
       <c r="B127" t="s">
+        <v>162</v>
+      </c>
+      <c r="C127" t="s">
         <v>54</v>
       </c>
-      <c r="C127" s="1">
+      <c r="D127" s="1">
         <v>45563</v>
       </c>
-      <c r="D127">
-        <v>0</v>
-      </c>
-      <c r="F127" t="s">
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="G127" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>103</v>
       </c>
       <c r="B128" t="s">
+        <v>162</v>
+      </c>
+      <c r="C128" t="s">
         <v>7</v>
       </c>
-      <c r="C128" s="1">
+      <c r="D128" s="1">
         <v>45563</v>
       </c>
-      <c r="D128">
-        <v>0</v>
-      </c>
-      <c r="F128" t="s">
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="G128" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>103</v>
       </c>
       <c r="B129" t="s">
+        <v>162</v>
+      </c>
+      <c r="C129" t="s">
         <v>9</v>
       </c>
-      <c r="C129" s="1">
+      <c r="D129" s="1">
         <v>45566</v>
       </c>
-      <c r="D129">
-        <v>0</v>
-      </c>
-      <c r="F129" t="s">
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="G129" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>103</v>
       </c>
       <c r="B130" t="s">
+        <v>162</v>
+      </c>
+      <c r="C130" t="s">
         <v>63</v>
       </c>
-      <c r="C130" s="1">
+      <c r="D130" s="1">
         <v>45560</v>
       </c>
-      <c r="D130">
-        <v>0</v>
-      </c>
-      <c r="F130" t="s">
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="G130" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>103</v>
       </c>
       <c r="B131" t="s">
+        <v>162</v>
+      </c>
+      <c r="C131" t="s">
         <v>11</v>
       </c>
-      <c r="C131" s="1">
+      <c r="D131" s="1">
         <v>45566</v>
       </c>
-      <c r="D131">
-        <v>0</v>
-      </c>
-      <c r="F131" t="s">
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="G131" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>103</v>
       </c>
       <c r="B132" t="s">
+        <v>162</v>
+      </c>
+      <c r="C132" t="s">
         <v>12</v>
       </c>
-      <c r="C132" s="1">
+      <c r="D132" s="1">
         <v>45566</v>
       </c>
-      <c r="D132">
-        <v>0</v>
-      </c>
-      <c r="F132" t="s">
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="G132" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>103</v>
       </c>
       <c r="B133" t="s">
+        <v>162</v>
+      </c>
+      <c r="C133" t="s">
         <v>13</v>
       </c>
-      <c r="C133" s="1">
+      <c r="D133" s="1">
         <v>45566</v>
       </c>
-      <c r="D133">
-        <v>0</v>
-      </c>
-      <c r="F133" t="s">
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="G133" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>103</v>
       </c>
       <c r="B134" t="s">
+        <v>162</v>
+      </c>
+      <c r="C134" t="s">
         <v>14</v>
       </c>
-      <c r="C134" s="1">
+      <c r="D134" s="1">
         <v>45566</v>
       </c>
-      <c r="D134">
-        <v>0</v>
-      </c>
-      <c r="F134" t="s">
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="G134" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>103</v>
       </c>
       <c r="B135" t="s">
+        <v>162</v>
+      </c>
+      <c r="C135" t="s">
         <v>16</v>
       </c>
-      <c r="C135" s="1">
+      <c r="D135" s="1">
         <v>45566</v>
       </c>
-      <c r="D135">
-        <v>0</v>
-      </c>
-      <c r="F135" t="s">
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="G135" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>103</v>
       </c>
       <c r="B136" t="s">
+        <v>162</v>
+      </c>
+      <c r="C136" t="s">
         <v>30</v>
       </c>
-      <c r="C136" s="1">
+      <c r="D136" s="1">
         <v>45569</v>
       </c>
-      <c r="D136">
-        <v>0</v>
-      </c>
-      <c r="F136" t="s">
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="G136" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>103</v>
       </c>
       <c r="B137" t="s">
+        <v>162</v>
+      </c>
+      <c r="C137" t="s">
         <v>32</v>
       </c>
-      <c r="C137" s="1">
+      <c r="D137" s="1">
         <v>45569</v>
       </c>
-      <c r="D137">
-        <v>0</v>
-      </c>
-      <c r="F137" t="s">
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="G137" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>103</v>
       </c>
       <c r="B138" t="s">
+        <v>162</v>
+      </c>
+      <c r="C138" t="s">
         <v>34</v>
       </c>
-      <c r="C138" s="1">
+      <c r="D138" s="1">
         <v>45569</v>
       </c>
-      <c r="D138">
-        <v>0</v>
-      </c>
-      <c r="F138" t="s">
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="G138" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>103</v>
       </c>
       <c r="B139" t="s">
+        <v>162</v>
+      </c>
+      <c r="C139" t="s">
         <v>35</v>
       </c>
-      <c r="C139" s="1">
+      <c r="D139" s="1">
         <v>45569</v>
       </c>
-      <c r="D139">
-        <v>0</v>
-      </c>
-      <c r="F139" t="s">
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="G139" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>103</v>
       </c>
       <c r="B140" t="s">
+        <v>162</v>
+      </c>
+      <c r="C140" t="s">
         <v>65</v>
       </c>
-      <c r="C140" s="1">
+      <c r="D140" s="1">
         <v>45560</v>
       </c>
-      <c r="D140">
-        <v>0</v>
-      </c>
-      <c r="F140" t="s">
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="G140" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>103</v>
       </c>
       <c r="B141" t="s">
+        <v>162</v>
+      </c>
+      <c r="C141" t="s">
         <v>37</v>
       </c>
-      <c r="C141" s="1">
+      <c r="D141" s="1">
         <v>45569</v>
       </c>
-      <c r="D141">
-        <v>0</v>
-      </c>
-      <c r="F141" t="s">
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="G141" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>103</v>
       </c>
       <c r="B142" t="s">
+        <v>162</v>
+      </c>
+      <c r="C142" t="s">
         <v>41</v>
       </c>
-      <c r="C142" s="1">
+      <c r="D142" s="1">
         <v>45569</v>
       </c>
-      <c r="D142">
-        <v>0</v>
-      </c>
-      <c r="F142" t="s">
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="G142" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>103</v>
       </c>
       <c r="B143" t="s">
+        <v>162</v>
+      </c>
+      <c r="C143" t="s">
         <v>38</v>
       </c>
-      <c r="C143" s="1">
+      <c r="D143" s="1">
         <v>45569</v>
       </c>
-      <c r="D143">
-        <v>0</v>
-      </c>
-      <c r="F143" t="s">
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="G143" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>103</v>
       </c>
       <c r="B144" t="s">
+        <v>162</v>
+      </c>
+      <c r="C144" t="s">
         <v>39</v>
       </c>
-      <c r="C144" s="1">
+      <c r="D144" s="1">
         <v>45569</v>
       </c>
-      <c r="D144">
-        <v>0</v>
-      </c>
-      <c r="F144" t="s">
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="G144" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>103</v>
       </c>
       <c r="B145" t="s">
+        <v>162</v>
+      </c>
+      <c r="C145" t="s">
         <v>40</v>
       </c>
-      <c r="C145" s="1">
+      <c r="D145" s="1">
         <v>45569</v>
       </c>
-      <c r="D145">
-        <v>0</v>
-      </c>
-      <c r="F145" t="s">
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="G145" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>103</v>
       </c>
       <c r="B146" t="s">
+        <v>162</v>
+      </c>
+      <c r="C146" t="s">
         <v>74</v>
       </c>
-      <c r="C146" s="1">
+      <c r="D146" s="1">
         <v>45569</v>
       </c>
-      <c r="D146">
-        <v>0</v>
-      </c>
-      <c r="F146" t="s">
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="G146" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>103</v>
       </c>
       <c r="B147" t="s">
+        <v>162</v>
+      </c>
+      <c r="C147" t="s">
         <v>55</v>
       </c>
-      <c r="C147" s="1">
+      <c r="D147" s="1">
         <v>45563</v>
       </c>
-      <c r="D147">
-        <v>0</v>
-      </c>
-      <c r="F147" t="s">
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="G147" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>103</v>
       </c>
       <c r="B148" t="s">
+        <v>162</v>
+      </c>
+      <c r="C148" t="s">
         <v>57</v>
       </c>
-      <c r="C148" s="1">
+      <c r="D148" s="1">
         <v>45563</v>
       </c>
-      <c r="D148">
-        <v>0</v>
-      </c>
-      <c r="F148" t="s">
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="G148" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>103</v>
       </c>
       <c r="B149" t="s">
+        <v>162</v>
+      </c>
+      <c r="C149" t="s">
         <v>150</v>
       </c>
-      <c r="C149" s="1">
+      <c r="D149" s="1">
         <v>45560</v>
       </c>
-      <c r="D149">
-        <v>0</v>
-      </c>
-      <c r="F149" t="s">
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="G149" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>103</v>
       </c>
       <c r="B150" t="s">
+        <v>162</v>
+      </c>
+      <c r="C150" t="s">
         <v>151</v>
       </c>
-      <c r="C150" s="1">
+      <c r="D150" s="1">
         <v>45560</v>
       </c>
-      <c r="D150">
-        <v>0</v>
-      </c>
-      <c r="F150" t="s">
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="G150" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>103</v>
       </c>
       <c r="B151" t="s">
+        <v>162</v>
+      </c>
+      <c r="C151" t="s">
         <v>66</v>
       </c>
-      <c r="C151" s="1">
+      <c r="D151" s="1">
         <v>45560</v>
       </c>
-      <c r="D151">
-        <v>0</v>
-      </c>
-      <c r="F151" t="s">
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="G151" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>103</v>
       </c>
       <c r="B152" t="s">
+        <v>162</v>
+      </c>
+      <c r="C152" t="s">
         <v>152</v>
       </c>
-      <c r="C152" s="1">
+      <c r="D152" s="1">
         <v>45560</v>
       </c>
-      <c r="D152">
-        <v>0</v>
-      </c>
-      <c r="F152" t="s">
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="G152" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>103</v>
       </c>
       <c r="B153" t="s">
+        <v>162</v>
+      </c>
+      <c r="C153" t="s">
         <v>153</v>
       </c>
-      <c r="C153" s="1">
+      <c r="D153" s="1">
         <v>45560</v>
       </c>
-      <c r="D153">
-        <v>0</v>
-      </c>
-      <c r="F153" t="s">
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="G153" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>103</v>
       </c>
       <c r="B154" t="s">
+        <v>162</v>
+      </c>
+      <c r="C154" t="s">
         <v>154</v>
       </c>
-      <c r="C154" s="1">
+      <c r="D154" s="1">
         <v>45563</v>
       </c>
-      <c r="D154">
-        <v>0</v>
-      </c>
-      <c r="F154" t="s">
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="G154" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>103</v>
       </c>
       <c r="B155" t="s">
+        <v>162</v>
+      </c>
+      <c r="C155" t="s">
         <v>59</v>
       </c>
-      <c r="C155" s="1">
+      <c r="D155" s="1">
         <v>45563</v>
       </c>
-      <c r="D155">
-        <v>0</v>
-      </c>
-      <c r="F155" t="s">
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="G155" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>103</v>
       </c>
       <c r="B156" t="s">
+        <v>162</v>
+      </c>
+      <c r="C156" t="s">
         <v>155</v>
       </c>
-      <c r="C156" s="1">
+      <c r="D156" s="1">
         <v>45560</v>
       </c>
-      <c r="D156">
-        <v>0</v>
-      </c>
-      <c r="F156" t="s">
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="G156" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>103</v>
       </c>
       <c r="B157" t="s">
+        <v>162</v>
+      </c>
+      <c r="C157" t="s">
         <v>44</v>
       </c>
-      <c r="C157" s="1">
+      <c r="D157" s="1">
         <v>45569</v>
       </c>
-      <c r="D157">
-        <v>0</v>
-      </c>
-      <c r="F157" t="s">
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="G157" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>103</v>
       </c>
       <c r="B158" t="s">
+        <v>162</v>
+      </c>
+      <c r="C158" t="s">
         <v>46</v>
       </c>
-      <c r="C158" s="1">
+      <c r="D158" s="1">
         <v>45933</v>
       </c>
-      <c r="D158">
-        <v>0</v>
-      </c>
-      <c r="F158" t="s">
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="G158" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>103</v>
       </c>
       <c r="B159" t="s">
+        <v>162</v>
+      </c>
+      <c r="C159" t="s">
         <v>17</v>
       </c>
-      <c r="C159" s="1">
+      <c r="D159" s="1">
         <v>45565</v>
       </c>
-      <c r="D159">
-        <v>0</v>
-      </c>
-      <c r="F159" t="s">
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="G159" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>103</v>
       </c>
       <c r="B160" t="s">
+        <v>162</v>
+      </c>
+      <c r="C160" t="s">
         <v>19</v>
       </c>
-      <c r="C160" s="1">
+      <c r="D160" s="1">
         <v>45565</v>
       </c>
-      <c r="D160">
-        <v>0</v>
-      </c>
-      <c r="F160" t="s">
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="G160" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>103</v>
       </c>
       <c r="B161" t="s">
+        <v>162</v>
+      </c>
+      <c r="C161" t="s">
         <v>67</v>
       </c>
-      <c r="C161" s="1">
+      <c r="D161" s="1">
         <v>45559</v>
       </c>
-      <c r="D161">
-        <v>1</v>
-      </c>
-      <c r="F161" t="s">
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="G161" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>103</v>
       </c>
       <c r="B162" t="s">
+        <v>162</v>
+      </c>
+      <c r="C162" t="s">
         <v>23</v>
       </c>
-      <c r="C162" s="1">
+      <c r="D162" s="1">
         <v>45565</v>
       </c>
-      <c r="D162">
-        <v>0</v>
-      </c>
-      <c r="F162" t="s">
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="G162" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>103</v>
       </c>
       <c r="B163" t="s">
+        <v>162</v>
+      </c>
+      <c r="C163" t="s">
         <v>24</v>
       </c>
-      <c r="C163" s="1">
+      <c r="D163" s="1">
         <v>45565</v>
       </c>
-      <c r="D163">
-        <v>1</v>
-      </c>
-      <c r="F163" t="s">
+      <c r="E163">
+        <v>1</v>
+      </c>
+      <c r="G163" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>103</v>
       </c>
       <c r="B164" t="s">
+        <v>162</v>
+      </c>
+      <c r="C164" t="s">
         <v>26</v>
       </c>
-      <c r="C164" s="1">
+      <c r="D164" s="1">
         <v>45565</v>
       </c>
-      <c r="D164">
-        <v>0</v>
-      </c>
-      <c r="F164" t="s">
+      <c r="E164">
+        <v>0</v>
+      </c>
+      <c r="G164" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>103</v>
       </c>
       <c r="B165" t="s">
+        <v>162</v>
+      </c>
+      <c r="C165" t="s">
         <v>28</v>
       </c>
-      <c r="C165" s="1">
+      <c r="D165" s="1">
         <v>45565</v>
       </c>
-      <c r="D165">
-        <v>0</v>
-      </c>
-      <c r="F165" t="s">
+      <c r="E165">
+        <v>0</v>
+      </c>
+      <c r="G165" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>103</v>
       </c>
       <c r="B166" t="s">
+        <v>162</v>
+      </c>
+      <c r="C166" t="s">
         <v>60</v>
       </c>
-      <c r="C166" s="1">
+      <c r="D166" s="1">
         <v>45563</v>
       </c>
-      <c r="D166">
-        <v>0</v>
-      </c>
-      <c r="F166" t="s">
+      <c r="E166">
+        <v>0</v>
+      </c>
+      <c r="G166" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>103</v>
       </c>
       <c r="B167" t="s">
+        <v>162</v>
+      </c>
+      <c r="C167" t="s">
         <v>68</v>
       </c>
-      <c r="C167" s="1">
+      <c r="D167" s="1">
         <v>45560</v>
       </c>
-      <c r="D167">
-        <v>0</v>
-      </c>
-      <c r="F167" t="s">
+      <c r="E167">
+        <v>0</v>
+      </c>
+      <c r="G167" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>103</v>
       </c>
       <c r="B168" t="s">
+        <v>162</v>
+      </c>
+      <c r="C168" t="s">
         <v>69</v>
       </c>
-      <c r="C168" s="1">
+      <c r="D168" s="1">
         <v>45560</v>
       </c>
-      <c r="D168">
-        <v>0</v>
-      </c>
-      <c r="F168" t="s">
+      <c r="E168">
+        <v>0</v>
+      </c>
+      <c r="G168" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>103</v>
       </c>
       <c r="B169" t="s">
+        <v>162</v>
+      </c>
+      <c r="C169" t="s">
         <v>71</v>
       </c>
-      <c r="C169" s="1">
+      <c r="D169" s="1">
         <v>45560</v>
       </c>
-      <c r="D169">
-        <v>0</v>
-      </c>
-      <c r="F169" t="s">
+      <c r="E169">
+        <v>0</v>
+      </c>
+      <c r="G169" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C170" s="1"/>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C171" s="1"/>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C172" s="1"/>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C173" s="1"/>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C174" s="1"/>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C175" s="1"/>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C176" s="1"/>
-    </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C177" s="1"/>
-    </row>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C178" s="1"/>
-    </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C179" s="1"/>
-    </row>
-    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C180" s="1"/>
-    </row>
-    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C181" s="1"/>
-    </row>
-    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C182" s="1"/>
-    </row>
-    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C183" s="1"/>
-    </row>
-    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C184" s="1"/>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D170" s="1"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D171" s="1"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D172" s="1"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D173" s="1"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D174" s="1"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D175" s="1"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D176" s="1"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D177" s="1"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D178" s="1"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D179" s="1"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D180" s="1"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D181" s="1"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D182" s="1"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D183" s="1"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D184" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1">
-    <sortState ref="A2:F117">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>